<commit_message>
Removed Two cem crt files
</commit_message>
<xml_diff>
--- a/Database-Architecture.xlsx
+++ b/Database-Architecture.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayankku\OneDrive - AMDOCS\Backup Folders\Desktop\Personal\Imagine-Penguins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="524" documentId="8_{EAC40BDB-1E30-4E81-97E6-1D7CB66DA9FD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{FAB381A5-32A3-4748-AB02-A9E152C1664F}"/>
+  <xr:revisionPtr revIDLastSave="730" documentId="8_{EAC40BDB-1E30-4E81-97E6-1D7CB66DA9FD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{F189096D-A152-4FF9-99F7-D2BB2BBAF008}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1BA3C163-F237-4EA7-AE1C-C550F94B9D6C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Users" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="171">
   <si>
     <t>name</t>
   </si>
@@ -40,15 +40,6 @@
     <t>Address</t>
   </si>
   <si>
-    <t>EmailTypes</t>
-  </si>
-  <si>
-    <t>PhoneTypes</t>
-  </si>
-  <si>
-    <t>Users</t>
-  </si>
-  <si>
     <t>address_1</t>
   </si>
   <si>
@@ -112,9 +103,6 @@
     <t>country_name</t>
   </si>
   <si>
-    <t>UserPhone</t>
-  </si>
-  <si>
     <t>phone_type_id</t>
   </si>
   <si>
@@ -124,39 +112,21 @@
     <t>last_name</t>
   </si>
   <si>
-    <t>UserEmail</t>
-  </si>
-  <si>
     <t>email_type_id</t>
   </si>
   <si>
-    <t>Picture</t>
-  </si>
-  <si>
     <t>picture_id</t>
   </si>
   <si>
     <t>picture_desc</t>
   </si>
   <si>
-    <t>PictureType</t>
-  </si>
-  <si>
-    <t>picture_type_id</t>
-  </si>
-  <si>
-    <t>picture_type_desc</t>
-  </si>
-  <si>
     <t>picture_path</t>
   </si>
   <si>
     <t>active</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -196,9 +166,6 @@
     <t>institution_type_desc</t>
   </si>
   <si>
-    <t>InstitutionPhone</t>
-  </si>
-  <si>
     <t>InstitutionEmail</t>
   </si>
   <si>
@@ -247,9 +214,6 @@
     <t>Teacher: Head of department, Class Teacher, Subject Teachers</t>
   </si>
   <si>
-    <t>Employee</t>
-  </si>
-  <si>
     <t>employee_type_id</t>
   </si>
   <si>
@@ -259,48 +223,21 @@
     <t>employee_type_desc</t>
   </si>
   <si>
-    <t>Teachers</t>
-  </si>
-  <si>
     <t>teacher_id</t>
   </si>
   <si>
-    <t>teacher_type_desc</t>
-  </si>
-  <si>
-    <t>teacher_type_name</t>
-  </si>
-  <si>
-    <t>Student</t>
-  </si>
-  <si>
-    <t>Role</t>
-  </si>
-  <si>
     <t>students</t>
   </si>
   <si>
     <t>student</t>
   </si>
   <si>
-    <t>role_id</t>
-  </si>
-  <si>
     <t>teacher</t>
   </si>
   <si>
-    <t>role_type</t>
-  </si>
-  <si>
-    <t>role_desc</t>
-  </si>
-  <si>
     <t>parent</t>
   </si>
   <si>
-    <t>Parent</t>
-  </si>
-  <si>
     <t>User types are: Employee, Students, Parents</t>
   </si>
   <si>
@@ -400,9 +337,6 @@
     <t>gender</t>
   </si>
   <si>
-    <t>DOB</t>
-  </si>
-  <si>
     <t>blood_group</t>
   </si>
   <si>
@@ -476,13 +410,148 @@
   </si>
   <si>
     <t>class_rep_type_desc</t>
+  </si>
+  <si>
+    <t>class_section</t>
+  </si>
+  <si>
+    <t>class_section_id</t>
+  </si>
+  <si>
+    <t>subject_skill</t>
+  </si>
+  <si>
+    <t>subject_skill_id</t>
+  </si>
+  <si>
+    <t>skill_name</t>
+  </si>
+  <si>
+    <t>skill_id</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>skill_desc</t>
+  </si>
+  <si>
+    <t>skills_id</t>
+  </si>
+  <si>
+    <t>parent_id</t>
+  </si>
+  <si>
+    <t>Create School</t>
+  </si>
+  <si>
+    <t>Add Employees</t>
+  </si>
+  <si>
+    <t>Select Type(Teaching|Non Teaching)</t>
+  </si>
+  <si>
+    <t>Add Batch</t>
+  </si>
+  <si>
+    <t>Add Courses|Class</t>
+  </si>
+  <si>
+    <t>Create Shift</t>
+  </si>
+  <si>
+    <t>reporting_manager</t>
+  </si>
+  <si>
+    <t>heirarchy</t>
+  </si>
+  <si>
+    <t>heirarchy_id</t>
+  </si>
+  <si>
+    <t>intitution_id</t>
+  </si>
+  <si>
+    <t>designation</t>
+  </si>
+  <si>
+    <t>student_id</t>
+  </si>
+  <si>
+    <t>college_activity_name</t>
+  </si>
+  <si>
+    <t>college_activity_id</t>
+  </si>
+  <si>
+    <t>college_activities(Event)</t>
+  </si>
+  <si>
+    <t>parents_student</t>
+  </si>
+  <si>
+    <t>parents_student_id</t>
+  </si>
+  <si>
+    <t>institution_classes</t>
+  </si>
+  <si>
+    <t>institution_classes_id</t>
+  </si>
+  <si>
+    <t>institution_class_teacher</t>
+  </si>
+  <si>
+    <t>institution_class_teacher_id</t>
+  </si>
+  <si>
+    <t>class_subject</t>
+  </si>
+  <si>
+    <t>class_subject_id</t>
+  </si>
+  <si>
+    <t>deleted_time</t>
+  </si>
+  <si>
+    <t>unique_QR_code</t>
+  </si>
+  <si>
+    <t>is_admin</t>
+  </si>
+  <si>
+    <t>is_super_admin</t>
+  </si>
+  <si>
+    <t>user_email</t>
+  </si>
+  <si>
+    <t>users</t>
+  </si>
+  <si>
+    <t>user_phones</t>
+  </si>
+  <si>
+    <t>email_types</t>
+  </si>
+  <si>
+    <t>phone_types</t>
+  </si>
+  <si>
+    <t>institution_phone</t>
+  </si>
+  <si>
+    <t>display_pic</t>
+  </si>
+  <si>
+    <t>display_pic_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -499,6 +568,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
@@ -527,11 +605,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -846,25 +925,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF1404B9-F0CB-4C7C-A240-0F224889816A}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" customWidth="1"/>
     <col min="8" max="8" width="28.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
     <col min="10" max="10" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
@@ -872,594 +950,742 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>49</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>167</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>166</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>164</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>168</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>165</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="I2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="L2" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" t="s">
-        <v>36</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>58</v>
+        <v>47</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" t="s">
-        <v>37</v>
+        <v>22</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L4" t="s">
         <v>29</v>
-      </c>
-      <c r="I4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" t="s">
-        <v>59</v>
-      </c>
-      <c r="L4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="I5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="K5" t="s">
-        <v>60</v>
-      </c>
-      <c r="L5" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>13</v>
+        <v>170</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="H8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="G8" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>66</v>
+        <v>41</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>41</v>
+        <v>31</v>
+      </c>
+      <c r="H9" t="s">
+        <v>37</v>
       </c>
       <c r="I9" t="s">
-        <v>42</v>
+        <v>32</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" t="s">
-        <v>65</v>
+        <v>42</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="I10" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="J10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F11" t="s">
+        <v>160</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" t="s">
+        <v>99</v>
+      </c>
+      <c r="H12" t="s">
+        <v>77</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" t="s">
+        <v>78</v>
+      </c>
+      <c r="K13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" t="s">
         <v>61</v>
       </c>
-      <c r="E11" t="s">
-        <v>67</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="1" t="s">
+      <c r="F14" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="G14" t="s">
+        <v>101</v>
+      </c>
+      <c r="H14" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" t="s">
+        <v>104</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J15" t="s">
+        <v>91</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" t="s">
+        <v>124</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="J16" t="s">
+        <v>92</v>
+      </c>
+      <c r="K16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" t="s">
+        <v>161</v>
+      </c>
+      <c r="H17" t="s">
+        <v>113</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J17" t="s">
+        <v>125</v>
+      </c>
+      <c r="K17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H18" t="s">
+        <v>114</v>
+      </c>
+      <c r="I18" t="s">
+        <v>123</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" t="s">
         <v>120</v>
       </c>
-      <c r="J12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G13" t="s">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E19" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" t="s">
+        <v>158</v>
+      </c>
+      <c r="H19" t="s">
+        <v>103</v>
+      </c>
+      <c r="I19" t="s">
+        <v>105</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" t="s">
+        <v>154</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J20" t="s">
+        <v>116</v>
+      </c>
+      <c r="K20" t="s">
         <v>121</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G14" t="s">
-        <v>123</v>
-      </c>
-      <c r="H14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D15" t="s">
-        <v>90</v>
-      </c>
-      <c r="F15" t="s">
-        <v>94</v>
-      </c>
-      <c r="G15" t="s">
-        <v>126</v>
-      </c>
-      <c r="H15" t="s">
-        <v>47</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" t="s">
-        <v>146</v>
-      </c>
-      <c r="I16" t="s">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H23" t="s">
+        <v>152</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>156</v>
+      </c>
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
+        <v>144</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="I25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
         <v>99</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="C28" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29" t="s">
+        <v>129</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>115</v>
-      </c>
-      <c r="C17" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J17" s="1"/>
-      <c r="K17" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>116</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E18" t="s">
-        <v>73</v>
-      </c>
-      <c r="H18" t="s">
-        <v>98</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+      <c r="I30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="I31" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
         <v>124</v>
       </c>
-      <c r="E19" t="s">
-        <v>74</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H19" t="s">
-        <v>96</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J19" t="s">
-        <v>112</v>
-      </c>
-      <c r="K19" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>130</v>
-      </c>
-      <c r="D20" t="s">
-        <v>125</v>
-      </c>
-      <c r="G20" t="s">
-        <v>56</v>
-      </c>
-      <c r="H20" t="s">
-        <v>97</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="J20" t="s">
-        <v>113</v>
-      </c>
-      <c r="K20" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>132</v>
-      </c>
-      <c r="G21" t="s">
-        <v>13</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="J21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C22" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G22" t="s">
-        <v>58</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
-        <v>134</v>
-      </c>
-      <c r="D23" t="s">
-        <v>106</v>
-      </c>
-      <c r="F23" t="s">
-        <v>105</v>
-      </c>
-      <c r="G23" t="s">
-        <v>29</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I23" t="s">
-        <v>145</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C24" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D24" t="s">
-        <v>110</v>
-      </c>
-      <c r="F24" t="s">
-        <v>108</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" t="s">
-        <v>135</v>
-      </c>
-      <c r="I24" t="s">
-        <v>127</v>
-      </c>
-      <c r="J24" t="s">
-        <v>138</v>
-      </c>
-      <c r="K24" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C25" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H25" t="s">
-        <v>136</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="K25" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G26" t="s">
-        <v>39</v>
-      </c>
-      <c r="H26" t="s">
-        <v>125</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K26" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G27" t="s">
-        <v>40</v>
-      </c>
-      <c r="K27" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G28" t="s">
-        <v>41</v>
-      </c>
-      <c r="K28" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G29" t="s">
-        <v>42</v>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1470,112 +1696,86 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A20A68-AACC-4822-AB5F-371105E56E8D}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="68.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>88</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
+      <c r="B8" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" t="s">
+        <v>141</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1583,6 +1783,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002B581E38B833EE4EA77B6B79D0C24E49" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="118743c08561cd65477a2e67d885b332">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="020cb9b8-a057-4ebb-8545-974d49b079a5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="05738d49843fb01ef453299c69d82f4d" ns1:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1783,25 +2001,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C89AFA86-4958-4D51-9AB3-F9B95F470685}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F097F7-CD2B-42F9-9D9F-198C20C0B2F1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DA868BC-499F-4D9E-A998-B23F3A7E9E47}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1818,22 +2036,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F097F7-CD2B-42F9-9D9F-198C20C0B2F1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C89AFA86-4958-4D51-9AB3-F9B95F470685}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>